<commit_message>
MVP v1 : Inventory Scraping, Stock uses dropdown
</commit_message>
<xml_diff>
--- a/P1/in/Inventory.xlsx
+++ b/P1/in/Inventory.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Wk of 02-20-2023" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Inventory" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -470,7 +470,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C2" s="0" t="n">
-        <x:v>979</x:v>
+        <x:v>249</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
@@ -481,7 +481,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C3" s="0" t="n">
-        <x:v>-29</x:v>
+        <x:v>787</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
@@ -492,7 +492,7 @@
         <x:v>9.5</x:v>
       </x:c>
       <x:c r="C4" s="0" t="n">
-        <x:v>84</x:v>
+        <x:v>1537</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
@@ -503,7 +503,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C5" s="0" t="n">
-        <x:v>1643</x:v>
+        <x:v>1251</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
@@ -514,7 +514,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C6" s="0" t="n">
-        <x:v>1567</x:v>
+        <x:v>1210</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
@@ -525,7 +525,7 @@
         <x:v>10.68</x:v>
       </x:c>
       <x:c r="C7" s="0" t="n">
-        <x:v>1723</x:v>
+        <x:v>1382</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
@@ -536,7 +536,7 @@
         <x:v>131.75</x:v>
       </x:c>
       <x:c r="C8" s="0" t="n">
-        <x:v>953</x:v>
+        <x:v>472</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
@@ -547,7 +547,7 @@
         <x:v>7.75</x:v>
       </x:c>
       <x:c r="C9" s="0" t="n">
-        <x:v>1458</x:v>
+        <x:v>594</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
@@ -558,7 +558,7 @@
         <x:v>12.5</x:v>
       </x:c>
       <x:c r="C10" s="0" t="n">
-        <x:v>1563</x:v>
+        <x:v>1255</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
@@ -569,7 +569,7 @@
         <x:v>2.25</x:v>
       </x:c>
       <x:c r="C11" s="0" t="n">
-        <x:v>930</x:v>
+        <x:v>610</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
@@ -580,7 +580,7 @@
         <x:v>9.73</x:v>
       </x:c>
       <x:c r="C12" s="0" t="n">
-        <x:v>1705</x:v>
+        <x:v>1187</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
@@ -591,7 +591,7 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="C13" s="0" t="n">
-        <x:v>893</x:v>
+        <x:v>679</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
@@ -602,7 +602,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C14" s="0" t="n">
-        <x:v>1760</x:v>
+        <x:v>1387</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
@@ -613,7 +613,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C15" s="0" t="n">
-        <x:v>998</x:v>
+        <x:v>807</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
@@ -624,7 +624,7 @@
         <x:v>10.53</x:v>
       </x:c>
       <x:c r="C16" s="0" t="n">
-        <x:v>1000</x:v>
+        <x:v>537</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
@@ -635,7 +635,7 @@
         <x:v>8.5</x:v>
       </x:c>
       <x:c r="C17" s="0" t="n">
-        <x:v>1949</x:v>
+        <x:v>1681</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
@@ -646,7 +646,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C18" s="0" t="n">
-        <x:v>1651</x:v>
+        <x:v>871</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
@@ -657,7 +657,7 @@
         <x:v>6.5</x:v>
       </x:c>
       <x:c r="C19" s="0" t="n">
-        <x:v>1909</x:v>
+        <x:v>1622</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
@@ -668,7 +668,7 @@
         <x:v>7.5</x:v>
       </x:c>
       <x:c r="C20" s="0" t="n">
-        <x:v>1023</x:v>
+        <x:v>645</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
@@ -679,7 +679,7 @@
         <x:v>3.88</x:v>
       </x:c>
       <x:c r="C21" s="0" t="n">
-        <x:v>1863</x:v>
+        <x:v>1565</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
@@ -690,7 +690,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C22" s="0" t="n">
-        <x:v>987</x:v>
+        <x:v>755</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
@@ -701,7 +701,7 @@
         <x:v>14.25</x:v>
       </x:c>
       <x:c r="C23" s="0" t="n">
-        <x:v>1613</x:v>
+        <x:v>1476</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
@@ -712,7 +712,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C24" s="0" t="n">
-        <x:v>756</x:v>
+        <x:v>400</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
@@ -723,7 +723,7 @@
         <x:v>21.95</x:v>
       </x:c>
       <x:c r="C25" s="0" t="n">
-        <x:v>979</x:v>
+        <x:v>1795</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
MVP V2 Scrape Inventory and Apply Purchase Amount at checkout
</commit_message>
<xml_diff>
--- a/P1/in/Inventory.xlsx
+++ b/P1/in/Inventory.xlsx
@@ -470,7 +470,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C2" s="0" t="n">
-        <x:v>249</x:v>
+        <x:v>1971</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
@@ -481,7 +481,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C3" s="0" t="n">
-        <x:v>787</x:v>
+        <x:v>704</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
@@ -492,7 +492,7 @@
         <x:v>9.5</x:v>
       </x:c>
       <x:c r="C4" s="0" t="n">
-        <x:v>1537</x:v>
+        <x:v>1469</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
@@ -503,7 +503,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C5" s="0" t="n">
-        <x:v>1251</x:v>
+        <x:v>1114</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
@@ -514,7 +514,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C6" s="0" t="n">
-        <x:v>1210</x:v>
+        <x:v>1166</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
@@ -525,7 +525,7 @@
         <x:v>10.68</x:v>
       </x:c>
       <x:c r="C7" s="0" t="n">
-        <x:v>1382</x:v>
+        <x:v>1365</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
@@ -536,7 +536,7 @@
         <x:v>131.75</x:v>
       </x:c>
       <x:c r="C8" s="0" t="n">
-        <x:v>472</x:v>
+        <x:v>377</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
@@ -547,7 +547,7 @@
         <x:v>7.75</x:v>
       </x:c>
       <x:c r="C9" s="0" t="n">
-        <x:v>594</x:v>
+        <x:v>426</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
@@ -558,7 +558,7 @@
         <x:v>12.5</x:v>
       </x:c>
       <x:c r="C10" s="0" t="n">
-        <x:v>1255</x:v>
+        <x:v>1188</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
@@ -569,7 +569,7 @@
         <x:v>2.25</x:v>
       </x:c>
       <x:c r="C11" s="0" t="n">
-        <x:v>610</x:v>
+        <x:v>518</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
@@ -580,7 +580,7 @@
         <x:v>9.73</x:v>
       </x:c>
       <x:c r="C12" s="0" t="n">
-        <x:v>1187</x:v>
+        <x:v>1013</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
@@ -602,7 +602,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C14" s="0" t="n">
-        <x:v>1387</x:v>
+        <x:v>1261</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
@@ -613,7 +613,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C15" s="0" t="n">
-        <x:v>807</x:v>
+        <x:v>697</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
@@ -624,7 +624,7 @@
         <x:v>10.53</x:v>
       </x:c>
       <x:c r="C16" s="0" t="n">
-        <x:v>537</x:v>
+        <x:v>461</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
@@ -635,7 +635,7 @@
         <x:v>8.5</x:v>
       </x:c>
       <x:c r="C17" s="0" t="n">
-        <x:v>1681</x:v>
+        <x:v>1601</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
@@ -646,7 +646,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C18" s="0" t="n">
-        <x:v>871</x:v>
+        <x:v>685</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
@@ -657,7 +657,7 @@
         <x:v>6.5</x:v>
       </x:c>
       <x:c r="C19" s="0" t="n">
-        <x:v>1622</x:v>
+        <x:v>1542</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
@@ -668,7 +668,7 @@
         <x:v>7.5</x:v>
       </x:c>
       <x:c r="C20" s="0" t="n">
-        <x:v>645</x:v>
+        <x:v>535</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
@@ -679,7 +679,7 @@
         <x:v>3.88</x:v>
       </x:c>
       <x:c r="C21" s="0" t="n">
-        <x:v>1565</x:v>
+        <x:v>1483</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
@@ -690,7 +690,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C22" s="0" t="n">
-        <x:v>755</x:v>
+        <x:v>724</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
@@ -701,7 +701,7 @@
         <x:v>14.25</x:v>
       </x:c>
       <x:c r="C23" s="0" t="n">
-        <x:v>1476</x:v>
+        <x:v>1446</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
@@ -712,7 +712,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C24" s="0" t="n">
-        <x:v>400</x:v>
+        <x:v>285</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
@@ -723,7 +723,7 @@
         <x:v>21.95</x:v>
       </x:c>
       <x:c r="C25" s="0" t="n">
-        <x:v>1795</x:v>
+        <x:v>1677</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>